<commit_message>
"fix KNL export data"
</commit_message>
<xml_diff>
--- a/E-Learning/App_Data/ThongKeKQua_KNL.xlsx
+++ b/E-Learning/App_Data/ThongKeKQua_KNL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hoaphatcomvn-my.sharepoint.com/personal/phuocnv1_hoaphat_com_vn/Documents/Working/Software/ELEARNING_DEV/KNL/E-Learning/App_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - hoaphat.com.vn\Software\ELEARNING_DEV\ELearningWeb\E-Learning\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{2AFC2619-A3A0-440C-A243-F047841B7B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB49A3E0-D073-422C-9853-AAA18D052CD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A9C62-028A-41A6-B3E9-846F93A9A410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60E312A9-B38A-4080-82C8-0F62C17AC0BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{60E312A9-B38A-4080-82C8-0F62C17AC0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="NhanVien_KNL" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -83,17 +83,74 @@
     <t>Chưa đánh giá</t>
   </si>
   <si>
-    <t>Ngày đánh giá gần nhất</t>
-  </si>
-  <si>
     <t>Không đánh giá</t>
+  </si>
+  <si>
+    <t>Kết quả tự đánh giá</t>
+  </si>
+  <si>
+    <t>Số lượng năng lực</t>
+  </si>
+  <si>
+    <t>Ngày tự đánh giá lần gần nhất</t>
+  </si>
+  <si>
+    <t>Kết quả thẩm định</t>
+  </si>
+  <si>
+    <t>Kết quả phê duyệt</t>
+  </si>
+  <si>
+    <t>Ngày phê duyệt kết quả đánh giá gần nhất</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Điều kiện hoàn thành
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2 điều kiện
++ Ngày phê duyệt kết quả đánh giá lần gần nhất thuộc quý đó
++ Tổng Số lượng năng lực bị quá hạn của các loại năng lực = 0</t>
+    </r>
+  </si>
+  <si>
+    <t>Năng lực Không đạt</t>
+  </si>
+  <si>
+    <t>Năng lực Đạt</t>
+  </si>
+  <si>
+    <t>Năng lực Vượt yêu cầu</t>
+  </si>
+  <si>
+    <t>Năng lực Chưa đánh giá</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Số lượng năng lực bị quá hạn
+(Đếm bao nhiêu năng lực &gt; 90 ngày)</t>
+  </si>
+  <si>
+    <t>Số lượng năng lực bị quá hạn
+(Đếm bao nhiêu năng lực &gt; 180 ngày)</t>
+  </si>
+  <si>
+    <t>Kết quả phổ biến (XX/YY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +174,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -133,12 +201,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -162,36 +230,82 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,9 +324,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -250,7 +364,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -356,7 +470,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -498,7 +612,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBD710F-664C-4EDA-B7A0-B52FF52E5DC4}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,94 +635,265 @@
     <col min="9" max="9" width="36.28515625" customWidth="1"/>
     <col min="10" max="10" width="33.42578125" customWidth="1"/>
     <col min="11" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" customWidth="1"/>
-    <col min="17" max="17" width="28.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="33" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:33" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="7"/>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:33" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="4"/>
+    </row>
+    <row r="4" spans="1:33" ht="171" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="U4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="V4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
+  <mergeCells count="27">
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="X2:AE2"/>
+    <mergeCell ref="AF2:AF4"/>
+    <mergeCell ref="AG2:AG4"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update ket qua thong ke KNL
</commit_message>
<xml_diff>
--- a/E-Learning/App_Data/ThongKeKQua_KNL.xlsx
+++ b/E-Learning/App_Data/ThongKeKQua_KNL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - hoaphat.com.vn\Software\ELEARNING_DEV\ELearningWeb\E-Learning\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A9C62-028A-41A6-B3E9-846F93A9A410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B21BB-BD05-4820-9FA9-AF6119299E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{60E312A9-B38A-4080-82C8-0F62C17AC0BD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{60E312A9-B38A-4080-82C8-0F62C17AC0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="NhanVien_KNL" sheetId="1" r:id="rId1"/>
@@ -273,17 +273,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,16 +293,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -622,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBD710F-664C-4EDA-B7A0-B52FF52E5DC4}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,233 +639,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="6"/>
     </row>
-    <row r="2" spans="1:33" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2" t="s">
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2" t="s">
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="2" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2" t="s">
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="X3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2" t="s">
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2" t="s">
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2" t="s">
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="4"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="8"/>
     </row>
-    <row r="4" spans="1:33" ht="171" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="3" t="s">
+    <row r="4" spans="1:33" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="7"/>
+      <c r="S4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="T4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="V4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="3" t="s">
+      <c r="W4" s="7"/>
+      <c r="X4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AB4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AD4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AE4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="4"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
     <mergeCell ref="L2:L4"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="A1:AG1"/>
@@ -883,17 +893,6 @@
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>